<commit_message>
quel que ajustement pour cette journner
</commit_message>
<xml_diff>
--- a/public/preinscriptionexcel/PreInscriptionsEtudiant.xlsx
+++ b/public/preinscriptionexcel/PreInscriptionsEtudiant.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>John Doe</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>AGO Arnaud</t>
+  </si>
+  <si>
+    <t>jean</t>
   </si>
 </sst>
 </file>
@@ -1015,13 +1018,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="3"/>
   <cols>
     <col min="2" max="2" width="12.8888888888889"/>
     <col min="3" max="3" width="34.2222222222222" customWidth="1"/>
@@ -1055,7 +1058,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" ht="15.15" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1094,6 +1097,20 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>67347422</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>